<commit_message>
fishing entrance, exit, verify without hardware
</commit_message>
<xml_diff>
--- a/app/python_logic/usuarios.xlsx
+++ b/app/python_logic/usuarios.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Nombre</t>
   </si>
@@ -25,7 +25,7 @@
     <t>Correo</t>
   </si>
   <si>
-    <t>102020120</t>
+    <t>1020810810</t>
   </si>
   <si>
     <t>wallace</t>
@@ -34,13 +34,19 @@
     <t>wallas</t>
   </si>
   <si>
-    <t>30343323222</t>
+    <t>Wilson Fabio</t>
+  </si>
+  <si>
+    <t>31200029299</t>
   </si>
   <si>
     <t>wia@c.com</t>
   </si>
   <si>
     <t>w@c.com</t>
+  </si>
+  <si>
+    <t>w@f.com</t>
   </si>
 </sst>
 </file>
@@ -398,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -426,21 +432,35 @@
         <v>302323222</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
+      <c r="A3" s="1">
+        <v>102020120</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>30343323222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>